<commit_message>
- CHG: Updated pedigree templates to include dataset information.
</commit_message>
<xml_diff>
--- a/pedigree-data/example-pedigree-data.xlsx
+++ b/pedigree-data/example-pedigree-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate\datatemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\pedigree-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672D2134-2BAE-40DA-9F15-4AE7B6ABD94E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BD3B80-F446-4783-BBBB-3B1FA7693E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="66">
   <si>
     <t>Pedigree Notation</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>ACCENUMB</t>
   </si>
   <si>
@@ -53,18 +50,12 @@
     <t>Information</t>
   </si>
   <si>
-    <t>If the pedigree string is available. This can be provided in the "DATA-STRING" sheet.</t>
-  </si>
-  <si>
     <t>Pedigree string</t>
   </si>
   <si>
     <t>Description of Crossing Procedure (if applicable)</t>
   </si>
   <si>
-    <t>The "DATA" sheet contains information about the two parents of a line/germplasm. If known, the first one should be the female parent and the second the male parent. If this is not known, the order doesn't matter.</t>
-  </si>
-  <si>
     <t>Help and Assistance</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
   </si>
   <si>
     <t>CACTUAR-6 * CACTUAR-6</t>
-  </si>
-  <si>
-    <t>Two types of pedigree information can be provided (Pedigree strings into sheet 'DATA-STRING' or atomised pedigree definitions into sheet 'DATA'). In all cases the MCPD field "ACCENUMB" should be used to identify the line/germplasm.</t>
   </si>
   <si>
     <r>
@@ -166,12 +154,94 @@
       <t>germinate@hutton.ac.uk</t>
     </r>
   </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>DEFINITION</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>A name given to the resource. Typically, a Title will be a name by which the resource is formally known.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>An account of the resource. Description may include but is not limited to: an abstract, a table of contents, a graphical representation, or a free-text account of the resource.</t>
+  </si>
+  <si>
+    <t>Rights</t>
+  </si>
+  <si>
+    <t>Information about rights held in and over the resource. Typically, rights information includes a statement about various property rights associated with the resource, including intellectual property rights.</t>
+  </si>
+  <si>
+    <t>Date of creation</t>
+  </si>
+  <si>
+    <t>A point or period of time associated with an event in the lifecycle of the resource. Date may be used to express temporal information at any level of granularity. Recommended best practice is to use an encoding scheme, such as the W3CDTF profile of ISO 8601 [W3CDTF].</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>An entity responsible for making the resource available. Examples of a Publisher include a person, an organization, or a service. Typically, the name of a Publisher should be used to indicate the entity.</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>The file format, physical medium, or dimensions of the resource. Examples of dimensions include size and duration. Recommended best practice is to use a controlled vocabulary such as the list of Internet Media Types [MIME].</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>A language of the resource. Recommended best practice is to use a controlled vocabulary such as RFC 4646 [RFC4646].</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>A related resource from which the described resource is derived. The described resource may be derived from the related resource in whole or in part. Recommended best practice is to identify the related resource by means of a string conforming to a formal identification system.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>The nature or genre of the resource. Recommended best practice is to use a controlled vocabulary such as the DCMI Type Vocabulary [DCMITYPE]. To describe the file format, physical medium, or dimensions of the resource, use the Format element.</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>The topic of the resource. Typically, the subject will be represented using keywords, key phrases, or classification codes. Recommended best practice is to use a controlled vocabulary.</t>
+  </si>
+  <si>
+    <t>The individual that can be contacted about this dataset.</t>
+  </si>
+  <si>
+    <t>Two types of pedigree information can be provided (Pedigree strings into sheet 'DATA-STRING' or atomised pedigree definitions into sheet 'DATA'). In all cases the MCPD field "ACCENUMB" should be used to identify the line/germplasm.
+If the pedigree string is available. This can be provided in the "DATA-STRING" sheet.</t>
+  </si>
+  <si>
+    <t>Pedigree data public version</t>
+  </si>
+  <si>
+    <t>Public version of the internal pedigree data. Contains a subset  of the whole pedigree.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,19 +278,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -300,47 +379,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -408,6 +497,106 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
       </font>
@@ -431,8 +620,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -447,6 +636,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{38AAE396-DAE3-432C-B66D-FEFDB8CC9188}" name="Table7" displayName="Table7" ref="A1:C12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:C12" xr:uid="{38AAE396-DAE3-432C-B66D-FEFDB8CC9188}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9A1BC290-1337-4F43-91E2-D79DE3424EC1}" name="LABEL" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E8E62A11-9DD3-4334-A6B4-B5C61CC4A5E5}" name="DEFINITION" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{420849A2-1140-4663-B890-CBF2E0537926}" name="VALUE" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0">
   <autoFilter ref="A1:F7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
@@ -461,7 +662,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:C13" totalsRowShown="0">
   <autoFilter ref="A1:C13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
@@ -473,7 +674,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:D7" totalsRowShown="0">
   <autoFilter ref="A1:D7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
@@ -486,7 +687,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table25" displayName="Table25" ref="A1:C13" totalsRowShown="0">
   <autoFilter ref="A1:C13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
@@ -761,70 +962,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="99.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="B12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="12"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
+      <formula>LEN(TRIM(C2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -847,142 +1164,142 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>23</v>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>23</v>
+      <c r="E7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C13"/>
     </sheetView>
   </sheetViews>
@@ -1017,10 +1334,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1028,134 +1345,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1192,167 +1509,167 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>23</v>
+      <c r="E5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>23</v>
+      <c r="E7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -1390,10 +1707,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1401,134 +1718,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>